<commit_message>
Alterado responsável do IPM_ELE.XLSX
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IPM_ELE.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IPM_ELE.XLSX
@@ -334,10 +334,10 @@
 MANUTENÇÃO ELÉTRICA</t>
   </si>
   <si>
-    <t>VALDECIR P DA SILVA</t>
-  </si>
-  <si>
-    <t>Matr.: 1330</t>
+    <t>GERSON DE ANDRADE</t>
+  </si>
+  <si>
+    <t>Matr.: 2777</t>
   </si>
   <si>
     <t>IPM_ELE</t>

</xml_diff>